<commit_message>
Padam Inputs TS6&7 and GS 6 05/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.2 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7D471C-9F5C-44BE-8B11-A460D8130B5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4968B5-8487-424A-8F8F-305AD3C7FE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4336,9 +4336,6 @@
     <t>dhUqrq.ShAqhAqviti# dhUH - sAqhauq</t>
   </si>
   <si>
-    <t>SB &amp;  etc'</t>
-  </si>
-  <si>
     <t>PS-5.17</t>
   </si>
   <si>
@@ -4394,6 +4391,9 @@
   </si>
   <si>
     <t>dura#H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SB </t>
   </si>
 </sst>
 </file>
@@ -5014,7 +5014,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1467" sqref="N1467"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5046,7 +5046,7 @@
         <v>62</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>1435</v>
+        <v>1454</v>
       </c>
       <c r="C1" s="40" t="s">
         <v>0</v>
@@ -5100,7 +5100,7 @@
         <v>189</v>
       </c>
       <c r="T1" s="68" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="U1" s="63" t="s">
         <v>16</v>
@@ -10983,7 +10983,7 @@
       <c r="E184" s="12"/>
       <c r="F184" s="12"/>
       <c r="G184" s="12" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="H184" s="12" t="s">
         <v>1391</v>
@@ -11014,7 +11014,7 @@
       <c r="E185" s="12"/>
       <c r="F185" s="12"/>
       <c r="G185" s="12" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="H185" s="12" t="s">
         <v>1391</v>
@@ -11045,7 +11045,7 @@
       <c r="E186" s="12"/>
       <c r="F186" s="12"/>
       <c r="G186" s="12" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="H186" s="12" t="s">
         <v>1391</v>
@@ -13361,7 +13361,7 @@
     </row>
     <row r="267" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E267" s="76" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="F267" s="12"/>
       <c r="G267" s="12"/>
@@ -13390,7 +13390,7 @@
     </row>
     <row r="268" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E268" s="76" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="F268" s="12"/>
       <c r="G268" s="12"/>
@@ -13793,7 +13793,7 @@
     <row r="282" spans="4:23" ht="18" x14ac:dyDescent="0.25">
       <c r="E282" s="12"/>
       <c r="F282" s="12" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="G282" s="12"/>
       <c r="H282" s="12"/>
@@ -13825,7 +13825,7 @@
     <row r="283" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E283" s="12"/>
       <c r="F283" s="12" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="G283" s="12"/>
       <c r="H283" s="12"/>
@@ -17743,7 +17743,7 @@
     <row r="421" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E421" s="12"/>
       <c r="F421" s="12" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="G421" s="12"/>
       <c r="H421" s="12"/>
@@ -17772,7 +17772,7 @@
     <row r="422" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E422" s="12"/>
       <c r="F422" s="12" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="G422" s="12"/>
       <c r="H422" s="12"/>
@@ -22128,7 +22128,7 @@
     </row>
     <row r="577" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E577" s="12" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="F577" s="12"/>
       <c r="G577" s="12"/>
@@ -22157,7 +22157,7 @@
     </row>
     <row r="578" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E578" s="12" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="F578" s="12"/>
       <c r="G578" s="12"/>
@@ -22794,7 +22794,7 @@
       <c r="E600" s="12"/>
       <c r="F600" s="12"/>
       <c r="G600" s="12" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="H600" s="74" t="s">
         <v>1404</v>
@@ -22829,7 +22829,7 @@
       <c r="E601" s="12"/>
       <c r="F601" s="12"/>
       <c r="G601" s="12" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="H601" s="74" t="s">
         <v>1404</v>
@@ -26506,10 +26506,10 @@
     </row>
     <row r="728" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E728" s="12" t="s">
+        <v>1437</v>
+      </c>
+      <c r="F728" s="12" t="s">
         <v>1438</v>
-      </c>
-      <c r="F728" s="12" t="s">
-        <v>1439</v>
       </c>
       <c r="G728" s="12"/>
       <c r="H728" s="74" t="s">
@@ -26541,10 +26541,10 @@
     </row>
     <row r="729" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E729" s="12" t="s">
+        <v>1437</v>
+      </c>
+      <c r="F729" s="12" t="s">
         <v>1438</v>
-      </c>
-      <c r="F729" s="12" t="s">
-        <v>1439</v>
       </c>
       <c r="G729" s="12"/>
       <c r="H729" s="74" t="s">
@@ -26574,10 +26574,10 @@
     </row>
     <row r="730" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E730" s="12" t="s">
+        <v>1437</v>
+      </c>
+      <c r="F730" s="12" t="s">
         <v>1438</v>
-      </c>
-      <c r="F730" s="12" t="s">
-        <v>1439</v>
       </c>
       <c r="G730" s="12"/>
       <c r="H730" s="74" t="s">
@@ -26611,10 +26611,10 @@
     </row>
     <row r="731" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E731" s="12" t="s">
+        <v>1437</v>
+      </c>
+      <c r="F731" s="12" t="s">
         <v>1438</v>
-      </c>
-      <c r="F731" s="12" t="s">
-        <v>1439</v>
       </c>
       <c r="G731" s="12"/>
       <c r="H731" s="74" t="s">
@@ -28608,12 +28608,12 @@
     </row>
     <row r="800" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B800" s="4" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="E800" s="12"/>
       <c r="F800" s="12"/>
       <c r="G800" s="12" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="H800" s="74" t="s">
         <v>1411</v>
@@ -28646,12 +28646,12 @@
     </row>
     <row r="801" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B801" s="4" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="E801" s="12"/>
       <c r="F801" s="12"/>
       <c r="G801" s="12" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="H801" s="74" t="s">
         <v>1411</v>
@@ -28684,12 +28684,12 @@
     </row>
     <row r="802" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B802" s="4" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="E802" s="12"/>
       <c r="F802" s="12"/>
       <c r="G802" s="12" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="H802" s="31"/>
       <c r="I802" s="47" t="s">
@@ -29765,7 +29765,7 @@
         <v>810</v>
       </c>
       <c r="O839" s="13" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="V839" s="23"/>
       <c r="W839" s="4"/>
@@ -35641,7 +35641,7 @@
         <v>180</v>
       </c>
       <c r="E1049" s="12" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="F1049" s="12"/>
       <c r="G1049" s="12"/>
@@ -35674,7 +35674,7 @@
         <v>180</v>
       </c>
       <c r="E1050" s="12" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="F1050" s="12"/>
       <c r="G1050" s="12"/>
@@ -48011,7 +48011,7 @@
         <v>116</v>
       </c>
       <c r="N1466" s="25" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="O1466" s="13"/>
       <c r="V1466" s="23"/>
@@ -48095,7 +48095,7 @@
         <v>64</v>
       </c>
       <c r="D1469" s="11" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="E1469" s="12"/>
       <c r="F1469" s="12"/>
@@ -51847,7 +51847,7 @@
         <v>180</v>
       </c>
       <c r="E1586" s="4" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="I1586" s="47" t="s">
         <v>57</v>
@@ -51880,7 +51880,7 @@
         <v>180</v>
       </c>
       <c r="E1587" s="4" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="I1587" s="47" t="s">
         <v>57</v>
@@ -52214,7 +52214,7 @@
         <v>64</v>
       </c>
       <c r="G1598" s="4" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="H1598" s="74" t="s">
         <v>1425</v>
@@ -52243,13 +52243,13 @@
     </row>
     <row r="1599" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1599" s="4" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="C1599" s="4" t="s">
         <v>64</v>
       </c>
       <c r="G1599" s="4" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="H1599" s="74" t="s">
         <v>1425</v>
@@ -52284,7 +52284,7 @@
         <v>64</v>
       </c>
       <c r="G1600" s="4" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="H1600" s="74" t="s">
         <v>1425</v>
@@ -52798,7 +52798,7 @@
         <v>180</v>
       </c>
       <c r="E1618" s="4" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="H1618" s="74" t="s">
         <v>1426</v>
@@ -52834,7 +52834,7 @@
         <v>180</v>
       </c>
       <c r="E1619" s="4" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="H1619" s="74" t="s">
         <v>1426</v>
@@ -54363,10 +54363,10 @@
         <v>64</v>
       </c>
       <c r="D1674" s="11" t="s">
+        <v>1441</v>
+      </c>
+      <c r="G1674" s="4" t="s">
         <v>1442</v>
-      </c>
-      <c r="G1674" s="4" t="s">
-        <v>1443</v>
       </c>
       <c r="I1674" s="47" t="s">
         <v>59</v>
@@ -54395,10 +54395,10 @@
         <v>64</v>
       </c>
       <c r="D1675" s="11" t="s">
+        <v>1441</v>
+      </c>
+      <c r="G1675" s="4" t="s">
         <v>1442</v>
-      </c>
-      <c r="G1675" s="4" t="s">
-        <v>1443</v>
       </c>
       <c r="I1675" s="47" t="s">
         <v>59</v>
@@ -54430,10 +54430,10 @@
         <v>64</v>
       </c>
       <c r="D1676" s="11" t="s">
+        <v>1441</v>
+      </c>
+      <c r="G1676" s="4" t="s">
         <v>1442</v>
-      </c>
-      <c r="G1676" s="4" t="s">
-        <v>1443</v>
       </c>
       <c r="I1676" s="4" t="s">
         <v>59</v>
@@ -54902,7 +54902,6 @@
       <c r="W1691" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V1691" xr:uid="{89ADA671-A008-49FA-997E-3118EBC45351}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
TS 1.2 Files pushed 30/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.2 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92685299-EE71-43FC-8CD0-6A23192C3A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D93AC50-1E43-46B4-8FCD-B47904F367DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4960" uniqueCount="1453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4959" uniqueCount="1453">
   <si>
     <t>Passage</t>
   </si>
@@ -5021,9 +5021,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1691"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1563" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1564" sqref="T1564"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1593" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O1557" sqref="O1557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -50951,9 +50951,7 @@
       <c r="N1557" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="O1557" s="13" t="s">
-        <v>21</v>
-      </c>
+      <c r="O1557" s="79"/>
       <c r="V1557" s="23"/>
       <c r="W1557" s="4"/>
     </row>

</xml_diff>

<commit_message>
nmv 25 02 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.2 Padam Input Template.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4959" uniqueCount="1453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4960" uniqueCount="1453">
   <si>
     <t>Passage</t>
   </si>
@@ -4510,7 +4510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4737,6 +4737,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5020,9 +5023,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1691"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1598" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1607" sqref="N1607"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U267" sqref="U267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13393,6 +13396,9 @@
         <v>415</v>
       </c>
       <c r="O267" s="13"/>
+      <c r="U267" s="81" t="s">
+        <v>70</v>
+      </c>
       <c r="V267" s="23"/>
       <c r="W267" s="4"/>
     </row>

</xml_diff>

<commit_message>
TS 1.1 to 1.6 Pada Paatam Corrections - 20/8/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.2 Padam Input Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CB51EB-BB6A-4B5C-BBC1-B5D4EF1F2C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 1.2" sheetId="1" r:id="rId1"/>
@@ -4389,7 +4390,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5026,11 +5027,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1691"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1404" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N1696" sqref="N1696"/>
     </sheetView>
   </sheetViews>
@@ -54928,7 +54929,7 @@
       <c r="W1691" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V1691"/>
+  <autoFilter ref="A1:V1691" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
nmv 02 11 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.2 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3F60D5-13A1-45A8-AAC1-F8FDC6171591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238D72B1-55DD-41D4-BD44-8D0CDCEDE955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3499,9 +3499,6 @@
     <t>kRuqNuqShvaq</t>
   </si>
   <si>
-    <t>daivyA#nI</t>
-  </si>
-  <si>
     <t>sthiqrA</t>
   </si>
   <si>
@@ -3679,9 +3676,6 @@
     <t>uqpaqyAti#</t>
   </si>
   <si>
-    <t>uqpaqyAtityu#pa - yAti#</t>
-  </si>
-  <si>
     <t>vasu#matA</t>
   </si>
   <si>
@@ -4052,9 +4046,6 @@
   </si>
   <si>
     <t>uqlkAH</t>
-  </si>
-  <si>
-    <t>ada#bdaH</t>
   </si>
   <si>
     <t>tiqgmaqheqteq</t>
@@ -4585,6 +4576,64 @@
         <family val="2"/>
       </rPr>
       <t>ndra - GoqShaH</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ada#b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>dha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>daivyA#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ni</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>uqpaqyA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>tIt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>yu#pa - yAti#</t>
     </r>
   </si>
 </sst>
@@ -5210,9 +5259,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1691"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1145" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V1148" sqref="V1148"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1527" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V1536" sqref="V1536"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5244,7 +5293,7 @@
         <v>62</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>1436</v>
+        <v>1433</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>0</v>
@@ -5298,7 +5347,7 @@
         <v>188</v>
       </c>
       <c r="T1" s="56" t="s">
-        <v>1434</v>
+        <v>1431</v>
       </c>
       <c r="U1" s="51" t="s">
         <v>16</v>
@@ -5958,7 +6007,7 @@
         <v>18</v>
       </c>
       <c r="N19" s="70" t="s">
-        <v>1441</v>
+        <v>1438</v>
       </c>
       <c r="O19" s="2" t="s">
         <v>21</v>
@@ -8343,7 +8392,7 @@
     </row>
     <row r="90" spans="1:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H90" s="4" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
       <c r="I90" s="4" t="s">
         <v>27</v>
@@ -8386,7 +8435,7 @@
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="4" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
       <c r="I91" s="4" t="s">
         <v>27</v>
@@ -8426,7 +8475,7 @@
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="4" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
       <c r="I92" s="4" t="s">
         <v>27</v>
@@ -8457,7 +8506,7 @@
     </row>
     <row r="93" spans="1:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H93" s="4" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
       <c r="I93" s="4" t="s">
         <v>27</v>
@@ -8597,7 +8646,7 @@
         <v>20</v>
       </c>
       <c r="V98" s="71" t="s">
-        <v>1442</v>
+        <v>1439</v>
       </c>
       <c r="W98" s="4"/>
     </row>
@@ -8719,7 +8768,7 @@
     </row>
     <row r="104" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H104" s="4" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="I104" s="4" t="s">
         <v>27</v>
@@ -8749,7 +8798,7 @@
     </row>
     <row r="105" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H105" s="4" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="I105" s="4" t="s">
         <v>27</v>
@@ -8774,7 +8823,7 @@
     </row>
     <row r="106" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H106" s="4" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="I106" s="4" t="s">
         <v>27</v>
@@ -8799,7 +8848,7 @@
     </row>
     <row r="107" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H107" s="4" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="I107" s="4" t="s">
         <v>27</v>
@@ -8824,7 +8873,7 @@
     </row>
     <row r="108" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H108" s="4" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="I108" s="4" t="s">
         <v>27</v>
@@ -8849,7 +8898,7 @@
     </row>
     <row r="109" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H109" s="4" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="I109" s="4" t="s">
         <v>27</v>
@@ -9801,7 +9850,7 @@
     </row>
     <row r="150" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H150" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I150" s="4" t="s">
         <v>28</v>
@@ -9826,7 +9875,7 @@
     </row>
     <row r="151" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H151" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I151" s="4" t="s">
         <v>28</v>
@@ -9858,7 +9907,7 @@
     </row>
     <row r="152" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H152" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I152" s="4" t="s">
         <v>28</v>
@@ -9888,7 +9937,7 @@
     </row>
     <row r="153" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H153" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I153" s="4" t="s">
         <v>28</v>
@@ -9913,7 +9962,7 @@
     </row>
     <row r="154" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H154" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I154" s="4" t="s">
         <v>28</v>
@@ -9943,7 +9992,7 @@
     </row>
     <row r="155" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H155" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I155" s="4" t="s">
         <v>28</v>
@@ -9968,7 +10017,7 @@
     </row>
     <row r="156" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H156" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I156" s="4" t="s">
         <v>28</v>
@@ -9996,7 +10045,7 @@
     </row>
     <row r="157" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H157" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I157" s="4" t="s">
         <v>28</v>
@@ -10021,7 +10070,7 @@
     </row>
     <row r="158" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H158" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I158" s="4" t="s">
         <v>28</v>
@@ -10051,7 +10100,7 @@
     </row>
     <row r="159" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H159" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I159" s="4" t="s">
         <v>28</v>
@@ -10076,7 +10125,7 @@
     </row>
     <row r="160" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H160" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I160" s="4" t="s">
         <v>29</v>
@@ -10101,7 +10150,7 @@
     </row>
     <row r="161" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H161" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I161" s="4" t="s">
         <v>29</v>
@@ -10129,7 +10178,7 @@
     </row>
     <row r="162" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H162" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I162" s="4" t="s">
         <v>29</v>
@@ -10154,7 +10203,7 @@
     </row>
     <row r="163" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H163" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I163" s="4" t="s">
         <v>29</v>
@@ -10179,7 +10228,7 @@
     </row>
     <row r="164" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H164" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I164" s="4" t="s">
         <v>29</v>
@@ -10209,7 +10258,7 @@
     </row>
     <row r="165" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H165" s="4" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="I165" s="4" t="s">
         <v>29</v>
@@ -10610,7 +10659,7 @@
     </row>
     <row r="182" spans="7:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H182" s="4" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="I182" s="4" t="s">
         <v>29</v>
@@ -10635,7 +10684,7 @@
     </row>
     <row r="183" spans="7:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H183" s="4" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="I183" s="4" t="s">
         <v>29</v>
@@ -10660,10 +10709,10 @@
     </row>
     <row r="184" spans="7:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G184" s="4" t="s">
-        <v>1428</v>
+        <v>1425</v>
       </c>
       <c r="H184" s="4" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="I184" s="4" t="s">
         <v>29</v>
@@ -10688,10 +10737,10 @@
     </row>
     <row r="185" spans="7:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G185" s="4" t="s">
-        <v>1428</v>
+        <v>1425</v>
       </c>
       <c r="H185" s="4" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="I185" s="4" t="s">
         <v>29</v>
@@ -10716,10 +10765,10 @@
     </row>
     <row r="186" spans="7:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G186" s="4" t="s">
-        <v>1428</v>
+        <v>1425</v>
       </c>
       <c r="H186" s="4" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="I186" s="4" t="s">
         <v>29</v>
@@ -10749,7 +10798,7 @@
     </row>
     <row r="187" spans="7:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H187" s="4" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="I187" s="4" t="s">
         <v>29</v>
@@ -10774,7 +10823,7 @@
     </row>
     <row r="188" spans="7:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H188" s="4" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="I188" s="4" t="s">
         <v>29</v>
@@ -10799,7 +10848,7 @@
     </row>
     <row r="189" spans="7:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H189" s="4" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="I189" s="4" t="s">
         <v>29</v>
@@ -11190,7 +11239,7 @@
         <v>96</v>
       </c>
       <c r="N205" s="71" t="s">
-        <v>1443</v>
+        <v>1440</v>
       </c>
       <c r="V205" s="20"/>
       <c r="W205" s="4"/>
@@ -11557,7 +11606,7 @@
     </row>
     <row r="221" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H221" s="61" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="I221" s="4" t="s">
         <v>30</v>
@@ -11583,7 +11632,7 @@
     </row>
     <row r="222" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H222" s="61" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="I222" s="4" t="s">
         <v>30</v>
@@ -11609,7 +11658,7 @@
     </row>
     <row r="223" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H223" s="61" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="I223" s="4" t="s">
         <v>30</v>
@@ -11634,7 +11683,7 @@
     </row>
     <row r="224" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H224" s="61" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="I224" s="4" t="s">
         <v>30</v>
@@ -11659,7 +11708,7 @@
     </row>
     <row r="225" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H225" s="61" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="I225" s="4" t="s">
         <v>30</v>
@@ -11687,7 +11736,7 @@
     </row>
     <row r="226" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H226" s="61" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="I226" s="4" t="s">
         <v>30</v>
@@ -11718,7 +11767,7 @@
     <row r="227" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D227" s="12"/>
       <c r="H227" s="61" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="I227" s="4" t="s">
         <v>30</v>
@@ -12285,7 +12334,7 @@
         <v>11</v>
       </c>
       <c r="N250" s="20" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="P250" s="18" t="s">
         <v>66</v>
@@ -12669,7 +12718,7 @@
     </row>
     <row r="267" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E267" s="63" t="s">
-        <v>1430</v>
+        <v>1427</v>
       </c>
       <c r="I267" s="4" t="s">
         <v>31</v>
@@ -12697,7 +12746,7 @@
     </row>
     <row r="268" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E268" s="63" t="s">
-        <v>1430</v>
+        <v>1427</v>
       </c>
       <c r="I268" s="4" t="s">
         <v>31</v>
@@ -13000,7 +13049,7 @@
         <v>41</v>
       </c>
       <c r="N280" s="20" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="P280" s="18" t="s">
         <v>66</v>
@@ -13035,7 +13084,7 @@
     </row>
     <row r="282" spans="4:23" ht="18" x14ac:dyDescent="0.25">
       <c r="F282" s="4" t="s">
-        <v>1432</v>
+        <v>1429</v>
       </c>
       <c r="I282" s="4" t="s">
         <v>31</v>
@@ -13064,7 +13113,7 @@
     </row>
     <row r="283" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F283" s="4" t="s">
-        <v>1432</v>
+        <v>1429</v>
       </c>
       <c r="I283" s="4" t="s">
         <v>31</v>
@@ -13274,7 +13323,7 @@
         <v>52</v>
       </c>
       <c r="N291" s="21" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="P291" s="18" t="s">
         <v>66</v>
@@ -13628,7 +13677,7 @@
     </row>
     <row r="306" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H306" s="61" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="I306" s="4" t="s">
         <v>32</v>
@@ -13654,7 +13703,7 @@
     </row>
     <row r="307" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H307" s="61" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="I307" s="4" t="s">
         <v>32</v>
@@ -13679,7 +13728,7 @@
     </row>
     <row r="308" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H308" s="61" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="I308" s="4" t="s">
         <v>32</v>
@@ -13704,7 +13753,7 @@
     </row>
     <row r="309" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H309" s="61" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="I309" s="4" t="s">
         <v>32</v>
@@ -13732,7 +13781,7 @@
     </row>
     <row r="310" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H310" s="61" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="I310" s="4" t="s">
         <v>32</v>
@@ -13757,7 +13806,7 @@
     </row>
     <row r="311" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H311" s="61" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="I311" s="4" t="s">
         <v>32</v>
@@ -13850,7 +13899,7 @@
     </row>
     <row r="315" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H315" s="61" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
       <c r="I315" s="4" t="s">
         <v>32</v>
@@ -13878,7 +13927,7 @@
     </row>
     <row r="316" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H316" s="61" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
       <c r="I316" s="4" t="s">
         <v>32</v>
@@ -13904,7 +13953,7 @@
     </row>
     <row r="317" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H317" s="61" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
       <c r="I317" s="4" t="s">
         <v>32</v>
@@ -13929,7 +13978,7 @@
     </row>
     <row r="318" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H318" s="61" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
       <c r="I318" s="4" t="s">
         <v>32</v>
@@ -13954,7 +14003,7 @@
     </row>
     <row r="319" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H319" s="61" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
       <c r="I319" s="4" t="s">
         <v>32</v>
@@ -14827,7 +14876,7 @@
     </row>
     <row r="358" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H358" s="61" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
       <c r="I358" s="4" t="s">
         <v>33</v>
@@ -14852,7 +14901,7 @@
     </row>
     <row r="359" spans="2:23" ht="18" x14ac:dyDescent="0.25">
       <c r="H359" s="61" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
       <c r="I359" s="4" t="s">
         <v>33</v>
@@ -14879,7 +14928,7 @@
     </row>
     <row r="360" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H360" s="61" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
       <c r="I360" s="4" t="s">
         <v>33</v>
@@ -14908,7 +14957,7 @@
     </row>
     <row r="361" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H361" s="61" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
       <c r="I361" s="4" t="s">
         <v>33</v>
@@ -14933,7 +14982,7 @@
     </row>
     <row r="362" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H362" s="61" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
       <c r="I362" s="4" t="s">
         <v>33</v>
@@ -15028,7 +15077,7 @@
         <v>21</v>
       </c>
       <c r="V365" s="71" t="s">
-        <v>1444</v>
+        <v>1441</v>
       </c>
       <c r="W365" s="4"/>
     </row>
@@ -15056,7 +15105,7 @@
     </row>
     <row r="367" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H367" s="61" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="I367" s="4" t="s">
         <v>33</v>
@@ -15081,7 +15130,7 @@
     </row>
     <row r="368" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H368" s="61" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="I368" s="4" t="s">
         <v>33</v>
@@ -15106,7 +15155,7 @@
     </row>
     <row r="369" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H369" s="61" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="I369" s="4" t="s">
         <v>33</v>
@@ -15131,7 +15180,7 @@
     </row>
     <row r="370" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H370" s="61" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="I370" s="4" t="s">
         <v>33</v>
@@ -15159,7 +15208,7 @@
     </row>
     <row r="371" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H371" s="61" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="I371" s="4" t="s">
         <v>33</v>
@@ -15184,7 +15233,7 @@
     </row>
     <row r="372" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H372" s="61" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="I372" s="4" t="s">
         <v>33</v>
@@ -15442,7 +15491,7 @@
     </row>
     <row r="383" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H383" s="61" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="I383" s="4" t="s">
         <v>33</v>
@@ -15472,7 +15521,7 @@
     </row>
     <row r="384" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H384" s="61" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="I384" s="4" t="s">
         <v>33</v>
@@ -15500,7 +15549,7 @@
         <v>180</v>
       </c>
       <c r="H385" s="61" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="I385" s="4" t="s">
         <v>33</v>
@@ -15528,7 +15577,7 @@
     </row>
     <row r="386" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H386" s="61" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="I386" s="4" t="s">
         <v>33</v>
@@ -15553,7 +15602,7 @@
     </row>
     <row r="387" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H387" s="61" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="I387" s="4" t="s">
         <v>33</v>
@@ -15578,7 +15627,7 @@
     </row>
     <row r="388" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H388" s="61" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="I388" s="4" t="s">
         <v>33</v>
@@ -15606,7 +15655,7 @@
     </row>
     <row r="389" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H389" s="61" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="I389" s="4" t="s">
         <v>33</v>
@@ -15631,7 +15680,7 @@
     </row>
     <row r="390" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H390" s="61" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="I390" s="4" t="s">
         <v>33</v>
@@ -15656,7 +15705,7 @@
     </row>
     <row r="391" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H391" s="61" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="I391" s="4" t="s">
         <v>33</v>
@@ -15684,7 +15733,7 @@
     </row>
     <row r="392" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H392" s="61" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="I392" s="4" t="s">
         <v>33</v>
@@ -15807,7 +15856,7 @@
     </row>
     <row r="397" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H397" s="61" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="I397" s="4" t="s">
         <v>33</v>
@@ -15835,7 +15884,7 @@
     </row>
     <row r="398" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H398" s="61" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="I398" s="4" t="s">
         <v>33</v>
@@ -15861,7 +15910,7 @@
     </row>
     <row r="399" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H399" s="61" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="I399" s="4" t="s">
         <v>33</v>
@@ -15886,7 +15935,7 @@
     </row>
     <row r="400" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H400" s="61" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="I400" s="4" t="s">
         <v>33</v>
@@ -16236,7 +16285,7 @@
         <v>175</v>
       </c>
       <c r="N414" s="20" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="P414" s="18" t="s">
         <v>66</v>
@@ -16380,7 +16429,7 @@
     </row>
     <row r="421" spans="6:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F421" s="4" t="s">
-        <v>1431</v>
+        <v>1428</v>
       </c>
       <c r="I421" s="4" t="s">
         <v>34</v>
@@ -16405,7 +16454,7 @@
     </row>
     <row r="422" spans="6:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F422" s="4" t="s">
-        <v>1431</v>
+        <v>1428</v>
       </c>
       <c r="I422" s="4" t="s">
         <v>34</v>
@@ -17032,7 +17081,7 @@
         <v>62</v>
       </c>
       <c r="H449" s="61" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="I449" s="4" t="s">
         <v>34</v>
@@ -17060,7 +17109,7 @@
         <v>62</v>
       </c>
       <c r="H450" s="61" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="I450" s="4" t="s">
         <v>34</v>
@@ -17088,7 +17137,7 @@
     </row>
     <row r="451" spans="1:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H451" s="61" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="I451" s="4" t="s">
         <v>34</v>
@@ -17113,7 +17162,7 @@
     </row>
     <row r="452" spans="1:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H452" s="61" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="I452" s="4" t="s">
         <v>34</v>
@@ -17492,7 +17541,7 @@
     </row>
     <row r="469" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H469" s="61" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="I469" s="4" t="s">
         <v>35</v>
@@ -17517,7 +17566,7 @@
     </row>
     <row r="470" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H470" s="61" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="I470" s="4" t="s">
         <v>35</v>
@@ -17543,7 +17592,7 @@
     </row>
     <row r="471" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H471" s="61" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="I471" s="4" t="s">
         <v>35</v>
@@ -17568,7 +17617,7 @@
     </row>
     <row r="472" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H472" s="61" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="I472" s="4" t="s">
         <v>35</v>
@@ -17598,7 +17647,7 @@
     </row>
     <row r="473" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H473" s="61" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="I473" s="4" t="s">
         <v>35</v>
@@ -17624,7 +17673,7 @@
     </row>
     <row r="474" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H474" s="61" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="I474" s="4" t="s">
         <v>35</v>
@@ -17664,7 +17713,7 @@
         <v>61</v>
       </c>
       <c r="N475" s="70" t="s">
-        <v>1445</v>
+        <v>1442</v>
       </c>
       <c r="O475" s="11" t="s">
         <v>21</v>
@@ -17691,7 +17740,7 @@
         <v>62</v>
       </c>
       <c r="N476" s="70" t="s">
-        <v>1446</v>
+        <v>1443</v>
       </c>
       <c r="O476" s="11" t="s">
         <v>21</v>
@@ -18283,7 +18332,7 @@
     </row>
     <row r="502" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H502" s="61" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="I502" s="4" t="s">
         <v>35</v>
@@ -18308,7 +18357,7 @@
     </row>
     <row r="503" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H503" s="61" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="I503" s="4" t="s">
         <v>35</v>
@@ -18333,7 +18382,7 @@
     </row>
     <row r="504" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H504" s="61" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="I504" s="4" t="s">
         <v>35</v>
@@ -18358,7 +18407,7 @@
     </row>
     <row r="505" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H505" s="61" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="I505" s="4" t="s">
         <v>35</v>
@@ -18383,7 +18432,7 @@
     </row>
     <row r="506" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H506" s="61" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="I506" s="4" t="s">
         <v>35</v>
@@ -18595,7 +18644,7 @@
         <v>181</v>
       </c>
       <c r="H515" s="61" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="I515" s="4" t="s">
         <v>35</v>
@@ -18626,7 +18675,7 @@
     </row>
     <row r="516" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H516" s="61" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="I516" s="4" t="s">
         <v>35</v>
@@ -18654,7 +18703,7 @@
     </row>
     <row r="517" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H517" s="61" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="I517" s="4" t="s">
         <v>35</v>
@@ -18679,7 +18728,7 @@
     </row>
     <row r="518" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H518" s="61" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="I518" s="4" t="s">
         <v>35</v>
@@ -18704,7 +18753,7 @@
     </row>
     <row r="519" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H519" s="61" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="I519" s="4" t="s">
         <v>35</v>
@@ -18722,7 +18771,7 @@
         <v>105</v>
       </c>
       <c r="N519" s="20" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="P519" s="18" t="s">
         <v>66</v>
@@ -19713,7 +19762,7 @@
         <v>43</v>
       </c>
       <c r="N562" s="20" t="s">
-        <v>1437</v>
+        <v>1434</v>
       </c>
       <c r="V562" s="20"/>
       <c r="W562" s="4"/>
@@ -20045,7 +20094,7 @@
     </row>
     <row r="577" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E577" s="4" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="I577" s="4" t="s">
         <v>37</v>
@@ -20070,10 +20119,10 @@
     </row>
     <row r="578" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E578" s="4" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="H578" s="61" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
       <c r="I578" s="4" t="s">
         <v>37</v>
@@ -20101,7 +20150,7 @@
     </row>
     <row r="579" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H579" s="61" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
       <c r="I579" s="4" t="s">
         <v>37</v>
@@ -20126,7 +20175,7 @@
     </row>
     <row r="580" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H580" s="61" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
       <c r="I580" s="4" t="s">
         <v>37</v>
@@ -20151,7 +20200,7 @@
     </row>
     <row r="581" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H581" s="61" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
       <c r="I581" s="4" t="s">
         <v>37</v>
@@ -20176,7 +20225,7 @@
     </row>
     <row r="582" spans="5:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H582" s="61" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
       <c r="I582" s="4" t="s">
         <v>37</v>
@@ -20216,7 +20265,7 @@
         <v>64</v>
       </c>
       <c r="N583" s="70" t="s">
-        <v>1447</v>
+        <v>1444</v>
       </c>
       <c r="V583" s="20"/>
       <c r="W583" s="4"/>
@@ -20565,7 +20614,7 @@
         <v>79</v>
       </c>
       <c r="N598" s="20" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="P598" s="18" t="s">
         <v>66</v>
@@ -20577,7 +20626,7 @@
     </row>
     <row r="599" spans="4:23" ht="18" x14ac:dyDescent="0.25">
       <c r="H599" s="61" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="I599" s="4" t="s">
         <v>38</v>
@@ -20606,10 +20655,10 @@
         <v>179</v>
       </c>
       <c r="G600" s="4" t="s">
-        <v>1423</v>
+        <v>1420</v>
       </c>
       <c r="H600" s="61" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="I600" s="4" t="s">
         <v>38</v>
@@ -20638,10 +20687,10 @@
         <v>179</v>
       </c>
       <c r="G601" s="4" t="s">
-        <v>1423</v>
+        <v>1420</v>
       </c>
       <c r="H601" s="61" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="I601" s="4" t="s">
         <v>38</v>
@@ -20827,7 +20876,7 @@
     </row>
     <row r="609" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H609" s="61" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="I609" s="4" t="s">
         <v>38</v>
@@ -20852,7 +20901,7 @@
     </row>
     <row r="610" spans="4:23" ht="18" x14ac:dyDescent="0.25">
       <c r="H610" s="61" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="I610" s="4" t="s">
         <v>38</v>
@@ -20882,7 +20931,7 @@
         <v>180</v>
       </c>
       <c r="H611" s="61" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="I611" s="4" t="s">
         <v>38</v>
@@ -20915,7 +20964,7 @@
     </row>
     <row r="612" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H612" s="61" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="I612" s="4" t="s">
         <v>38</v>
@@ -20940,7 +20989,7 @@
     </row>
     <row r="613" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H613" s="61" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="I613" s="4" t="s">
         <v>38</v>
@@ -21602,7 +21651,7 @@
         <v>41</v>
       </c>
       <c r="N639" s="20" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="P639" s="18" t="s">
         <v>66</v>
@@ -21767,7 +21816,7 @@
     </row>
     <row r="646" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H646" s="61" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="I646" s="4" t="s">
         <v>38</v>
@@ -21797,7 +21846,7 @@
     </row>
     <row r="647" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H647" s="61" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="I647" s="4" t="s">
         <v>38</v>
@@ -21826,7 +21875,7 @@
       </c>
       <c r="D648" s="62"/>
       <c r="H648" s="61" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="I648" s="4" t="s">
         <v>38</v>
@@ -21861,7 +21910,7 @@
     <row r="649" spans="2:23" ht="18" x14ac:dyDescent="0.25">
       <c r="D649" s="62"/>
       <c r="H649" s="61" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="I649" s="4" t="s">
         <v>38</v>
@@ -21892,7 +21941,7 @@
     <row r="650" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D650" s="62"/>
       <c r="H650" s="61" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="I650" s="4" t="s">
         <v>38</v>
@@ -22053,7 +22102,7 @@
         <v>57</v>
       </c>
       <c r="N655" s="20" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="P655" s="18" t="s">
         <v>66</v>
@@ -23229,7 +23278,7 @@
     </row>
     <row r="704" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H704" s="61" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="I704" s="4" t="s">
         <v>39</v>
@@ -23254,7 +23303,7 @@
     </row>
     <row r="705" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H705" s="61" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="I705" s="4" t="s">
         <v>39</v>
@@ -23279,7 +23328,7 @@
     </row>
     <row r="706" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H706" s="61" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="I706" s="4" t="s">
         <v>39</v>
@@ -23307,7 +23356,7 @@
     </row>
     <row r="707" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H707" s="61" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="I707" s="4" t="s">
         <v>39</v>
@@ -23332,7 +23381,7 @@
     </row>
     <row r="708" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H708" s="61" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="I708" s="4" t="s">
         <v>39</v>
@@ -23668,7 +23717,7 @@
     </row>
     <row r="722" spans="2:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H722" s="61" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="I722" s="4" t="s">
         <v>39</v>
@@ -23698,7 +23747,7 @@
     </row>
     <row r="723" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H723" s="61" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="I723" s="4" t="s">
         <v>39</v>
@@ -23722,14 +23771,14 @@
         <v>95</v>
       </c>
       <c r="T723" s="65" t="s">
-        <v>1370</v>
+        <v>1367</v>
       </c>
       <c r="V723" s="20"/>
       <c r="W723" s="4"/>
     </row>
     <row r="724" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H724" s="61" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="I724" s="4" t="s">
         <v>39</v>
@@ -23754,7 +23803,7 @@
     </row>
     <row r="725" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H725" s="61" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="I725" s="4" t="s">
         <v>39</v>
@@ -23822,7 +23871,7 @@
         <v>72</v>
       </c>
       <c r="N727" s="20" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="P727" s="18" t="s">
         <v>66</v>
@@ -23835,13 +23884,13 @@
     </row>
     <row r="728" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E728" s="4" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="F728" s="4" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
       <c r="H728" s="61" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="I728" s="4" t="s">
         <v>40</v>
@@ -23869,13 +23918,13 @@
     </row>
     <row r="729" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E729" s="4" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="F729" s="4" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
       <c r="H729" s="61" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="I729" s="4" t="s">
         <v>40</v>
@@ -23900,13 +23949,13 @@
     </row>
     <row r="730" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E730" s="4" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="F730" s="4" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
       <c r="H730" s="61" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="I730" s="4" t="s">
         <v>40</v>
@@ -23936,13 +23985,13 @@
     </row>
     <row r="731" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E731" s="4" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="F731" s="4" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
       <c r="H731" s="61" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="I731" s="4" t="s">
         <v>40</v>
@@ -23970,7 +24019,7 @@
     </row>
     <row r="732" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H732" s="61" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="I732" s="4" t="s">
         <v>40</v>
@@ -24747,7 +24796,7 @@
     </row>
     <row r="763" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H763" s="61" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="I763" s="4" t="s">
         <v>40</v>
@@ -24777,7 +24826,7 @@
     </row>
     <row r="764" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H764" s="61" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="I764" s="4" t="s">
         <v>40</v>
@@ -24802,7 +24851,7 @@
     </row>
     <row r="765" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H765" s="61" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="I765" s="4" t="s">
         <v>40</v>
@@ -24827,7 +24876,7 @@
     </row>
     <row r="766" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H766" s="61" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="I766" s="4" t="s">
         <v>40</v>
@@ -24852,7 +24901,7 @@
     </row>
     <row r="767" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H767" s="61" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="I767" s="4" t="s">
         <v>40</v>
@@ -25509,7 +25558,7 @@
         <v>66</v>
       </c>
       <c r="N793" s="20" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="P793" s="18" t="s">
         <v>66</v>
@@ -25595,7 +25644,7 @@
     </row>
     <row r="797" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H797" s="61" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="I797" s="4" t="s">
         <v>41</v>
@@ -25620,7 +25669,7 @@
     </row>
     <row r="798" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H798" s="61" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="I798" s="4" t="s">
         <v>41</v>
@@ -25648,7 +25697,7 @@
     </row>
     <row r="799" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H799" s="61" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="I799" s="4" t="s">
         <v>41</v>
@@ -25673,13 +25722,13 @@
     </row>
     <row r="800" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B800" s="4" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
       <c r="G800" s="4" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
       <c r="H800" s="61" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="I800" s="4" t="s">
         <v>41</v>
@@ -25697,25 +25746,25 @@
         <v>73</v>
       </c>
       <c r="N800" s="21" t="s">
-        <v>1414</v>
+        <v>1411</v>
       </c>
       <c r="O800" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V800" s="20" t="s">
-        <v>1417</v>
+        <v>1414</v>
       </c>
       <c r="W800" s="4"/>
     </row>
     <row r="801" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B801" s="4" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
       <c r="G801" s="4" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
       <c r="H801" s="61" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="I801" s="4" t="s">
         <v>41</v>
@@ -25745,10 +25794,10 @@
     </row>
     <row r="802" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B802" s="4" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
       <c r="G802" s="4" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
       <c r="H802" s="26"/>
       <c r="I802" s="4" t="s">
@@ -26017,7 +26066,7 @@
         <v>85</v>
       </c>
       <c r="N812" s="20" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="P812" s="18" t="s">
         <v>66</v>
@@ -26871,7 +26920,7 @@
         <v>35</v>
       </c>
       <c r="N847" s="70" t="s">
-        <v>1448</v>
+        <v>1445</v>
       </c>
       <c r="O847" s="11" t="s">
         <v>21</v>
@@ -27790,7 +27839,7 @@
         <v>73</v>
       </c>
       <c r="N885" s="20" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="P885" s="18" t="s">
         <v>66</v>
@@ -30234,7 +30283,7 @@
         <v>101</v>
       </c>
       <c r="N986" s="20" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="P986" s="18" t="s">
         <v>66</v>
@@ -30411,7 +30460,7 @@
     </row>
     <row r="993" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H993" s="61" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="I993" s="21" t="s">
         <v>45</v>
@@ -30436,7 +30485,7 @@
     </row>
     <row r="994" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H994" s="61" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="I994" s="21" t="s">
         <v>45</v>
@@ -30466,7 +30515,7 @@
     </row>
     <row r="995" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H995" s="61" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="I995" s="21" t="s">
         <v>45</v>
@@ -30494,7 +30543,7 @@
     </row>
     <row r="996" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H996" s="61" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="I996" s="21" t="s">
         <v>45</v>
@@ -30519,7 +30568,7 @@
     </row>
     <row r="997" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H997" s="61" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="I997" s="21" t="s">
         <v>45</v>
@@ -30954,7 +31003,7 @@
         <v>94</v>
       </c>
       <c r="T1014" s="18" t="s">
-        <v>1415</v>
+        <v>1412</v>
       </c>
       <c r="V1014" s="20"/>
       <c r="W1014" s="4"/>
@@ -31771,7 +31820,7 @@
         <v>179</v>
       </c>
       <c r="E1049" s="4" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="H1049" s="26"/>
       <c r="I1049" s="4" t="s">
@@ -31801,7 +31850,7 @@
         <v>179</v>
       </c>
       <c r="E1050" s="4" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="H1050" s="26"/>
       <c r="I1050" s="4" t="s">
@@ -32014,7 +32063,7 @@
     </row>
     <row r="1059" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1059" s="61" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="I1059" s="4" t="s">
         <v>46</v>
@@ -32039,7 +32088,7 @@
     </row>
     <row r="1060" spans="2:23" ht="18" x14ac:dyDescent="0.25">
       <c r="H1060" s="61" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="I1060" s="4" t="s">
         <v>46</v>
@@ -32067,7 +32116,7 @@
         <v>179</v>
       </c>
       <c r="H1061" s="61" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="I1061" s="4" t="s">
         <v>46</v>
@@ -32095,7 +32144,7 @@
     </row>
     <row r="1062" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1062" s="61" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="I1062" s="4" t="s">
         <v>46</v>
@@ -32125,7 +32174,7 @@
     </row>
     <row r="1063" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1063" s="61" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="I1063" s="4" t="s">
         <v>46</v>
@@ -32158,7 +32207,7 @@
         <v>61</v>
       </c>
       <c r="H1064" s="61" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="I1064" s="4" t="s">
         <v>46</v>
@@ -33466,7 +33515,7 @@
         <v>39</v>
       </c>
       <c r="N1115" s="71" t="s">
-        <v>1449</v>
+        <v>1446</v>
       </c>
       <c r="V1115" s="20"/>
       <c r="W1115" s="4"/>
@@ -33489,7 +33538,7 @@
         <v>40</v>
       </c>
       <c r="N1116" s="71" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
       <c r="V1116" s="20"/>
       <c r="W1116" s="4"/>
@@ -33852,7 +33901,7 @@
     </row>
     <row r="1132" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1132" s="61" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="I1132" s="4" t="s">
         <v>48</v>
@@ -33877,7 +33926,7 @@
     </row>
     <row r="1133" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1133" s="61" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="I1133" s="4" t="s">
         <v>48</v>
@@ -33902,7 +33951,7 @@
     </row>
     <row r="1134" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1134" s="61" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="I1134" s="4" t="s">
         <v>48</v>
@@ -33930,7 +33979,7 @@
         <v>60</v>
       </c>
       <c r="H1135" s="61" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="I1135" s="4" t="s">
         <v>48</v>
@@ -33959,7 +34008,7 @@
         <v>60</v>
       </c>
       <c r="H1136" s="61" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="I1136" s="4" t="s">
         <v>48</v>
@@ -33984,7 +34033,7 @@
     </row>
     <row r="1137" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1137" s="61" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="I1137" s="4" t="s">
         <v>48</v>
@@ -34009,7 +34058,7 @@
     </row>
     <row r="1138" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1138" s="61" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="I1138" s="4" t="s">
         <v>48</v>
@@ -34268,7 +34317,7 @@
         <v>21</v>
       </c>
       <c r="V1148" s="71" t="s">
-        <v>1451</v>
+        <v>1448</v>
       </c>
       <c r="W1148" s="4"/>
     </row>
@@ -35137,7 +35186,7 @@
     </row>
     <row r="1184" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1184" s="61" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="I1184" s="4" t="s">
         <v>49</v>
@@ -35162,7 +35211,7 @@
     </row>
     <row r="1185" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1185" s="61" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="I1185" s="4" t="s">
         <v>49</v>
@@ -35187,7 +35236,7 @@
     </row>
     <row r="1186" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1186" s="61" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="I1186" s="4" t="s">
         <v>49</v>
@@ -35215,7 +35264,7 @@
     </row>
     <row r="1187" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1187" s="61" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="I1187" s="4" t="s">
         <v>49</v>
@@ -35243,7 +35292,7 @@
         <v>61</v>
       </c>
       <c r="H1188" s="61" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="I1188" s="4" t="s">
         <v>49</v>
@@ -35269,7 +35318,7 @@
     </row>
     <row r="1189" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1189" s="61" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="I1189" s="4" t="s">
         <v>49</v>
@@ -35370,7 +35419,7 @@
     </row>
     <row r="1193" spans="2:23" ht="18" x14ac:dyDescent="0.25">
       <c r="C1193" s="4" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
       <c r="H1193" s="61" t="s">
         <v>87</v>
@@ -35403,7 +35452,7 @@
         <v>170</v>
       </c>
       <c r="C1194" s="4" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
       <c r="H1194" s="50" t="s">
         <v>87</v>
@@ -35433,7 +35482,7 @@
         <v>94</v>
       </c>
       <c r="T1194" s="18" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="V1194" s="20" t="s">
         <v>1002</v>
@@ -36050,7 +36099,7 @@
         <v>9</v>
       </c>
       <c r="N1220" s="20" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="P1220" s="18" t="s">
         <v>66</v>
@@ -36162,7 +36211,7 @@
     </row>
     <row r="1225" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1225" s="61" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="I1225" s="4" t="s">
         <v>50</v>
@@ -36187,7 +36236,7 @@
     </row>
     <row r="1226" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1226" s="61" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="I1226" s="4" t="s">
         <v>50</v>
@@ -36212,7 +36261,7 @@
     </row>
     <row r="1227" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1227" s="61" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="I1227" s="4" t="s">
         <v>50</v>
@@ -36237,7 +36286,7 @@
     </row>
     <row r="1228" spans="8:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1228" s="61" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="I1228" s="4" t="s">
         <v>50</v>
@@ -36307,7 +36356,7 @@
         <v>19</v>
       </c>
       <c r="N1230" s="21" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="O1230" s="11" t="s">
         <v>21</v>
@@ -36316,7 +36365,7 @@
         <v>66</v>
       </c>
       <c r="V1230" s="20" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="W1230" s="4"/>
     </row>
@@ -36828,7 +36877,7 @@
         <v>40</v>
       </c>
       <c r="N1251" s="20" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="P1251" s="18" t="s">
         <v>66</v>
@@ -37023,7 +37072,7 @@
         <v>48</v>
       </c>
       <c r="N1259" s="20" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="P1259" s="18" t="s">
         <v>66</v>
@@ -37278,7 +37327,7 @@
         <v>58</v>
       </c>
       <c r="N1269" s="21" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="O1269" s="11" t="s">
         <v>23</v>
@@ -37508,7 +37557,7 @@
         <v>67</v>
       </c>
       <c r="N1278" s="20" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="P1278" s="18" t="s">
         <v>66</v>
@@ -38241,7 +38290,7 @@
     </row>
     <row r="1309" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1309" s="61" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="I1309" s="4" t="s">
         <v>51</v>
@@ -38269,7 +38318,7 @@
     </row>
     <row r="1310" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1310" s="61" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="I1310" s="4" t="s">
         <v>51</v>
@@ -38297,7 +38346,7 @@
     </row>
     <row r="1311" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1311" s="61" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="I1311" s="4" t="s">
         <v>51</v>
@@ -38322,7 +38371,7 @@
     </row>
     <row r="1312" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1312" s="61" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="I1312" s="4" t="s">
         <v>52</v>
@@ -38347,7 +38396,7 @@
     </row>
     <row r="1313" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1313" s="61" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="I1313" s="4" t="s">
         <v>52</v>
@@ -38375,7 +38424,7 @@
     </row>
     <row r="1314" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1314" s="61" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="I1314" s="4" t="s">
         <v>52</v>
@@ -38400,7 +38449,7 @@
     </row>
     <row r="1315" spans="4:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1315" s="61" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="I1315" s="4" t="s">
         <v>52</v>
@@ -38418,7 +38467,7 @@
         <v>104</v>
       </c>
       <c r="N1315" s="20" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="P1315" s="18" t="s">
         <v>66</v>
@@ -39283,7 +39332,7 @@
         <v>64</v>
       </c>
       <c r="H1351" s="21" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="I1351" s="4" t="s">
         <v>53</v>
@@ -39311,7 +39360,7 @@
         <v>64</v>
       </c>
       <c r="H1352" s="21" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="I1352" s="4" t="s">
         <v>53</v>
@@ -39564,7 +39613,7 @@
         <v>10</v>
       </c>
       <c r="N1360" s="20" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="P1360" s="18" t="s">
         <v>66</v>
@@ -39691,7 +39740,7 @@
         <v>64</v>
       </c>
       <c r="H1365" s="21" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="I1365" s="4" t="s">
         <v>53</v>
@@ -39719,7 +39768,7 @@
         <v>64</v>
       </c>
       <c r="H1366" s="21" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="I1366" s="4" t="s">
         <v>53</v>
@@ -39747,7 +39796,7 @@
         <v>64</v>
       </c>
       <c r="H1367" s="21" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="I1367" s="4" t="s">
         <v>53</v>
@@ -39775,7 +39824,7 @@
         <v>64</v>
       </c>
       <c r="H1368" s="21" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="I1368" s="4" t="s">
         <v>53</v>
@@ -39803,7 +39852,7 @@
         <v>64</v>
       </c>
       <c r="H1369" s="21" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="I1369" s="4" t="s">
         <v>53</v>
@@ -39821,7 +39870,7 @@
         <v>19</v>
       </c>
       <c r="N1369" s="20" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P1369" s="18" t="s">
         <v>66</v>
@@ -40037,7 +40086,7 @@
         <v>27</v>
       </c>
       <c r="N1377" s="20" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="P1377" s="18" t="s">
         <v>66</v>
@@ -40295,7 +40344,7 @@
         <v>36</v>
       </c>
       <c r="N1386" s="20" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P1386" s="18" t="s">
         <v>66</v>
@@ -40578,8 +40627,8 @@
       <c r="M1396" s="7">
         <v>46</v>
       </c>
-      <c r="N1396" s="20" t="s">
-        <v>1341</v>
+      <c r="N1396" s="71" t="s">
+        <v>1449</v>
       </c>
       <c r="P1396" s="18" t="s">
         <v>66</v>
@@ -40712,7 +40761,7 @@
         <v>64</v>
       </c>
       <c r="H1401" s="21" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="I1401" s="4" t="s">
         <v>54</v>
@@ -40741,7 +40790,7 @@
         <v>64</v>
       </c>
       <c r="H1402" s="21" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="I1402" s="4" t="s">
         <v>54</v>
@@ -40772,7 +40821,7 @@
         <v>64</v>
       </c>
       <c r="H1403" s="21" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="I1403" s="4" t="s">
         <v>54</v>
@@ -40800,7 +40849,7 @@
         <v>64</v>
       </c>
       <c r="H1404" s="21" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="I1404" s="4" t="s">
         <v>54</v>
@@ -40824,7 +40873,7 @@
         <v>94</v>
       </c>
       <c r="T1404" s="57" t="s">
-        <v>1369</v>
+        <v>1366</v>
       </c>
       <c r="V1404" s="20"/>
       <c r="W1404" s="4"/>
@@ -40931,7 +40980,7 @@
         <v>58</v>
       </c>
       <c r="N1408" s="20" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="P1408" s="18" t="s">
         <v>66</v>
@@ -41231,7 +41280,7 @@
         <v>68</v>
       </c>
       <c r="N1418" s="21" t="s">
-        <v>1342</v>
+        <v>1339</v>
       </c>
       <c r="O1418" s="11" t="s">
         <v>21</v>
@@ -41240,7 +41289,7 @@
         <v>66</v>
       </c>
       <c r="V1418" s="20" t="s">
-        <v>1343</v>
+        <v>1340</v>
       </c>
       <c r="W1418" s="4"/>
     </row>
@@ -41533,7 +41582,7 @@
         <v>79</v>
       </c>
       <c r="N1429" s="20" t="s">
-        <v>1344</v>
+        <v>1341</v>
       </c>
       <c r="P1429" s="18" t="s">
         <v>66</v>
@@ -41600,7 +41649,7 @@
         <v>64</v>
       </c>
       <c r="H1432" s="61" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="I1432" s="4" t="s">
         <v>54</v>
@@ -41631,7 +41680,7 @@
         <v>64</v>
       </c>
       <c r="H1433" s="61" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="I1433" s="4" t="s">
         <v>54</v>
@@ -41659,7 +41708,7 @@
         <v>64</v>
       </c>
       <c r="H1434" s="61" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="I1434" s="4" t="s">
         <v>54</v>
@@ -41690,7 +41739,7 @@
         <v>64</v>
       </c>
       <c r="H1435" s="61" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="I1435" s="4" t="s">
         <v>54</v>
@@ -41718,7 +41767,7 @@
         <v>64</v>
       </c>
       <c r="H1436" s="61" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="I1436" s="4" t="s">
         <v>54</v>
@@ -41752,7 +41801,7 @@
         <v>64</v>
       </c>
       <c r="H1437" s="61" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="I1437" s="4" t="s">
         <v>54</v>
@@ -41796,8 +41845,8 @@
       <c r="M1438" s="7">
         <v>88</v>
       </c>
-      <c r="N1438" s="20" t="s">
-        <v>1156</v>
+      <c r="N1438" s="71" t="s">
+        <v>1450</v>
       </c>
       <c r="V1438" s="20"/>
       <c r="W1438" s="4"/>
@@ -41886,7 +41935,7 @@
         <v>91</v>
       </c>
       <c r="N1441" s="20" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="V1441" s="20"/>
       <c r="W1441" s="4"/>
@@ -41912,7 +41961,7 @@
         <v>92</v>
       </c>
       <c r="N1442" s="20" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="V1442" s="20"/>
       <c r="W1442" s="4"/>
@@ -41938,7 +41987,7 @@
         <v>93</v>
       </c>
       <c r="N1443" s="20" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="V1443" s="20"/>
       <c r="W1443" s="4"/>
@@ -41964,7 +42013,7 @@
         <v>94</v>
       </c>
       <c r="N1444" s="20" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="V1444" s="20"/>
       <c r="W1444" s="4"/>
@@ -41990,7 +42039,7 @@
         <v>95</v>
       </c>
       <c r="N1445" s="20" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="V1445" s="20"/>
       <c r="W1445" s="4"/>
@@ -42045,7 +42094,7 @@
         <v>97</v>
       </c>
       <c r="N1447" s="20" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="S1447" s="4"/>
       <c r="V1447" s="20"/>
@@ -42104,7 +42153,7 @@
         <v>99</v>
       </c>
       <c r="N1449" s="20" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="V1449" s="20"/>
       <c r="W1449" s="4"/>
@@ -42156,7 +42205,7 @@
         <v>101</v>
       </c>
       <c r="N1451" s="20" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="V1451" s="20"/>
       <c r="W1451" s="4"/>
@@ -42182,13 +42231,13 @@
         <v>102</v>
       </c>
       <c r="N1452" s="21" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="O1452" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1452" s="20" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="W1452" s="4"/>
     </row>
@@ -42213,7 +42262,7 @@
         <v>103</v>
       </c>
       <c r="N1453" s="20" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="V1453" s="20"/>
       <c r="W1453" s="4"/>
@@ -42265,7 +42314,7 @@
         <v>105</v>
       </c>
       <c r="N1455" s="20" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="V1455" s="20"/>
       <c r="W1455" s="4"/>
@@ -42291,7 +42340,7 @@
         <v>106</v>
       </c>
       <c r="N1456" s="20" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="V1456" s="20"/>
       <c r="W1456" s="4"/>
@@ -42317,7 +42366,7 @@
         <v>107</v>
       </c>
       <c r="N1457" s="20" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="V1457" s="20"/>
       <c r="W1457" s="4"/>
@@ -42343,7 +42392,7 @@
         <v>108</v>
       </c>
       <c r="N1458" s="20" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
       <c r="P1458" s="18" t="s">
         <v>66</v>
@@ -42400,7 +42449,7 @@
         <v>110</v>
       </c>
       <c r="N1460" s="20" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="V1460" s="20"/>
       <c r="W1460" s="4"/>
@@ -42426,13 +42475,13 @@
         <v>111</v>
       </c>
       <c r="N1461" s="21" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="O1461" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1461" s="20" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="W1461" s="4"/>
     </row>
@@ -42483,7 +42532,7 @@
         <v>113</v>
       </c>
       <c r="N1463" s="20" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="V1463" s="20"/>
       <c r="W1463" s="4"/>
@@ -42509,7 +42558,7 @@
         <v>114</v>
       </c>
       <c r="N1464" s="20" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="U1464" s="48" t="s">
         <v>70</v>
@@ -42567,7 +42616,7 @@
         <v>116</v>
       </c>
       <c r="N1466" s="20" t="s">
-        <v>1435</v>
+        <v>1432</v>
       </c>
       <c r="V1466" s="20"/>
       <c r="W1466" s="4"/>
@@ -42625,7 +42674,7 @@
         <v>118</v>
       </c>
       <c r="N1468" s="20" t="s">
-        <v>1346</v>
+        <v>1343</v>
       </c>
       <c r="P1468" s="18" t="s">
         <v>66</v>
@@ -42643,7 +42692,7 @@
         <v>64</v>
       </c>
       <c r="D1469" s="10" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
       <c r="H1469" s="26"/>
       <c r="I1469" s="4" t="s">
@@ -42662,7 +42711,7 @@
         <v>119</v>
       </c>
       <c r="N1469" s="20" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="S1469" s="32" t="s">
         <v>73</v>
@@ -42780,13 +42829,13 @@
         <v>123</v>
       </c>
       <c r="N1473" s="21" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="O1473" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1473" s="20" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="W1473" s="4"/>
     </row>
@@ -42811,13 +42860,13 @@
         <v>124</v>
       </c>
       <c r="N1474" s="21" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="O1474" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1474" s="20" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="W1474" s="4"/>
     </row>
@@ -42894,7 +42943,7 @@
         <v>127</v>
       </c>
       <c r="N1477" s="20" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="V1477" s="20"/>
       <c r="W1477" s="4"/>
@@ -42972,7 +43021,7 @@
         <v>130</v>
       </c>
       <c r="N1480" s="20" t="s">
-        <v>1347</v>
+        <v>1344</v>
       </c>
       <c r="P1480" s="18" t="s">
         <v>66</v>
@@ -43003,7 +43052,7 @@
         <v>131</v>
       </c>
       <c r="N1481" s="20" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="V1481" s="20"/>
       <c r="W1481" s="4"/>
@@ -43029,7 +43078,7 @@
         <v>132</v>
       </c>
       <c r="N1482" s="20" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="V1482" s="20"/>
       <c r="W1482" s="4"/>
@@ -43055,7 +43104,7 @@
         <v>133</v>
       </c>
       <c r="N1483" s="20" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="V1483" s="20"/>
       <c r="W1483" s="4"/>
@@ -43081,13 +43130,13 @@
         <v>134</v>
       </c>
       <c r="N1484" s="21" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="O1484" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1484" s="20" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="W1484" s="4"/>
     </row>
@@ -43164,7 +43213,7 @@
         <v>137</v>
       </c>
       <c r="N1487" s="20" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="V1487" s="20"/>
       <c r="W1487" s="4"/>
@@ -43190,13 +43239,13 @@
         <v>138</v>
       </c>
       <c r="N1488" s="21" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="O1488" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1488" s="20" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="W1488" s="4"/>
     </row>
@@ -43273,7 +43322,7 @@
         <v>141</v>
       </c>
       <c r="N1491" s="21" t="s">
-        <v>1438</v>
+        <v>1435</v>
       </c>
       <c r="P1491" s="18" t="s">
         <v>66</v>
@@ -43359,13 +43408,13 @@
         <v>144</v>
       </c>
       <c r="N1494" s="21" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="O1494" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1494" s="20" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="W1494" s="4"/>
     </row>
@@ -43390,7 +43439,7 @@
         <v>145</v>
       </c>
       <c r="N1495" s="20" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="V1495" s="20"/>
       <c r="W1495" s="4"/>
@@ -43419,7 +43468,7 @@
         <v>146</v>
       </c>
       <c r="N1496" s="20" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="S1496" s="4"/>
       <c r="V1496" s="20"/>
@@ -43501,7 +43550,7 @@
         <v>149</v>
       </c>
       <c r="N1499" s="20" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="V1499" s="20"/>
       <c r="W1499" s="4"/>
@@ -43527,7 +43576,7 @@
         <v>150</v>
       </c>
       <c r="N1500" s="20" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="V1500" s="20"/>
       <c r="W1500" s="4"/>
@@ -43579,7 +43628,7 @@
         <v>152</v>
       </c>
       <c r="N1502" s="20" t="s">
-        <v>1348</v>
+        <v>1345</v>
       </c>
       <c r="P1502" s="18" t="s">
         <v>66</v>
@@ -43610,13 +43659,13 @@
         <v>153</v>
       </c>
       <c r="N1503" s="21" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="O1503" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1503" s="20" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="W1503" s="4"/>
     </row>
@@ -43667,13 +43716,13 @@
         <v>155</v>
       </c>
       <c r="N1505" s="21" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="O1505" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1505" s="20" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="W1505" s="4"/>
     </row>
@@ -43698,7 +43747,7 @@
         <v>156</v>
       </c>
       <c r="N1506" s="20" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="U1506" s="48"/>
       <c r="V1506" s="20"/>
@@ -43759,7 +43808,7 @@
         <v>158</v>
       </c>
       <c r="N1508" s="20" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="V1508" s="20"/>
       <c r="W1508" s="4"/>
@@ -43785,7 +43834,7 @@
         <v>159</v>
       </c>
       <c r="N1509" s="20" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="V1509" s="20"/>
       <c r="W1509" s="4"/>
@@ -43840,7 +43889,7 @@
         <v>161</v>
       </c>
       <c r="N1511" s="20" t="s">
-        <v>1349</v>
+        <v>1346</v>
       </c>
       <c r="P1511" s="18" t="s">
         <v>66</v>
@@ -43923,7 +43972,7 @@
         <v>164</v>
       </c>
       <c r="N1514" s="20" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="V1514" s="20"/>
       <c r="W1514" s="4"/>
@@ -43978,7 +44027,7 @@
         <v>166</v>
       </c>
       <c r="N1516" s="20" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="V1516" s="20"/>
       <c r="W1516" s="4"/>
@@ -43988,7 +44037,7 @@
         <v>64</v>
       </c>
       <c r="H1517" s="61" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="I1517" s="4" t="s">
         <v>56</v>
@@ -44019,7 +44068,7 @@
         <v>64</v>
       </c>
       <c r="H1518" s="61" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="I1518" s="4" t="s">
         <v>56</v>
@@ -44037,7 +44086,7 @@
         <v>168</v>
       </c>
       <c r="N1518" s="21" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="V1518" s="20"/>
       <c r="W1518" s="4"/>
@@ -44048,7 +44097,7 @@
         <v>64</v>
       </c>
       <c r="H1519" s="61" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="I1519" s="4" t="s">
         <v>56</v>
@@ -44066,7 +44115,7 @@
         <v>169</v>
       </c>
       <c r="N1519" s="21" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="O1519" s="11" t="s">
         <v>21</v>
@@ -44078,7 +44127,7 @@
         <v>178</v>
       </c>
       <c r="V1519" s="20" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="W1519" s="4"/>
     </row>
@@ -44087,7 +44136,7 @@
         <v>64</v>
       </c>
       <c r="H1520" s="61" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="I1520" s="4" t="s">
         <v>56</v>
@@ -44105,7 +44154,7 @@
         <v>170</v>
       </c>
       <c r="N1520" s="20" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="V1520" s="20"/>
       <c r="W1520" s="4"/>
@@ -44115,7 +44164,7 @@
         <v>64</v>
       </c>
       <c r="H1521" s="61" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="I1521" s="4" t="s">
         <v>56</v>
@@ -44146,7 +44195,7 @@
         <v>64</v>
       </c>
       <c r="H1522" s="61" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="I1522" s="4" t="s">
         <v>56</v>
@@ -44164,7 +44213,7 @@
         <v>172</v>
       </c>
       <c r="N1522" s="20" t="s">
-        <v>1349</v>
+        <v>1346</v>
       </c>
       <c r="P1522" s="18" t="s">
         <v>66</v>
@@ -44195,7 +44244,7 @@
         <v>173</v>
       </c>
       <c r="N1523" s="20" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="V1523" s="20"/>
       <c r="W1523" s="4"/>
@@ -44249,13 +44298,13 @@
         <v>175</v>
       </c>
       <c r="N1525" s="21" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="O1525" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1525" s="20" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="W1525" s="4"/>
     </row>
@@ -44264,7 +44313,7 @@
         <v>64</v>
       </c>
       <c r="D1526" s="10" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="H1526" s="50" t="s">
         <v>90</v>
@@ -44285,7 +44334,7 @@
         <v>176</v>
       </c>
       <c r="N1526" s="20" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="S1526" s="2" t="s">
         <v>97</v>
@@ -44301,7 +44350,7 @@
         <v>64</v>
       </c>
       <c r="D1527" s="10" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="H1527" s="50" t="s">
         <v>90</v>
@@ -44354,7 +44403,7 @@
         <v>178</v>
       </c>
       <c r="N1528" s="20" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="V1528" s="20"/>
       <c r="W1528" s="4"/>
@@ -44379,7 +44428,7 @@
         <v>179</v>
       </c>
       <c r="N1529" s="20" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="V1529" s="20"/>
       <c r="W1529" s="4"/>
@@ -44404,7 +44453,7 @@
         <v>180</v>
       </c>
       <c r="N1530" s="20" t="s">
-        <v>1350</v>
+        <v>1347</v>
       </c>
       <c r="P1530" s="18" t="s">
         <v>66</v>
@@ -44484,13 +44533,13 @@
         <v>183</v>
       </c>
       <c r="N1533" s="21" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="O1533" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1533" s="20" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="W1533" s="4"/>
     </row>
@@ -44514,14 +44563,14 @@
         <v>184</v>
       </c>
       <c r="N1534" s="21" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="O1534" s="11" t="s">
         <v>21</v>
       </c>
       <c r="T1534" s="29"/>
       <c r="V1534" s="20" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="W1534" s="4"/>
     </row>
@@ -44573,13 +44622,13 @@
         <v>186</v>
       </c>
       <c r="N1536" s="21" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="O1536" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="V1536" s="20" t="s">
-        <v>1216</v>
+      <c r="V1536" s="71" t="s">
+        <v>1451</v>
       </c>
       <c r="W1536" s="4"/>
     </row>
@@ -44603,13 +44652,13 @@
         <v>187</v>
       </c>
       <c r="N1537" s="21" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="O1537" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1537" s="20" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="W1537" s="4"/>
     </row>
@@ -44633,7 +44682,7 @@
         <v>188</v>
       </c>
       <c r="N1538" s="20" t="s">
-        <v>1351</v>
+        <v>1348</v>
       </c>
       <c r="P1538" s="18" t="s">
         <v>66</v>
@@ -44688,7 +44737,7 @@
         <v>190</v>
       </c>
       <c r="N1540" s="20" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="V1540" s="20"/>
       <c r="W1540" s="4"/>
@@ -44713,7 +44762,7 @@
         <v>191</v>
       </c>
       <c r="N1541" s="20" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="V1541" s="20"/>
       <c r="W1541" s="4"/>
@@ -44863,7 +44912,7 @@
         <v>197</v>
       </c>
       <c r="N1547" s="20" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="V1547" s="20"/>
       <c r="W1547" s="4"/>
@@ -44888,7 +44937,7 @@
         <v>198</v>
       </c>
       <c r="N1548" s="20" t="s">
-        <v>1352</v>
+        <v>1349</v>
       </c>
       <c r="P1548" s="18" t="s">
         <v>66</v>
@@ -44943,7 +44992,7 @@
         <v>200</v>
       </c>
       <c r="N1550" s="20" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="V1550" s="20"/>
       <c r="W1550" s="4"/>
@@ -44968,7 +45017,7 @@
         <v>201</v>
       </c>
       <c r="N1551" s="20" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="V1551" s="20"/>
       <c r="W1551" s="4"/>
@@ -44993,13 +45042,13 @@
         <v>202</v>
       </c>
       <c r="N1552" s="21" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="O1552" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1552" s="20" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="W1552" s="4"/>
     </row>
@@ -45073,7 +45122,7 @@
         <v>205</v>
       </c>
       <c r="N1555" s="20" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="V1555" s="20"/>
       <c r="W1555" s="4"/>
@@ -45098,7 +45147,7 @@
         <v>206</v>
       </c>
       <c r="N1556" s="20" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="V1556" s="20"/>
       <c r="W1556" s="4"/>
@@ -45151,7 +45200,7 @@
         <v>208</v>
       </c>
       <c r="N1558" s="20" t="s">
-        <v>1353</v>
+        <v>1350</v>
       </c>
       <c r="P1558" s="18" t="s">
         <v>66</v>
@@ -45271,7 +45320,7 @@
         <v>212</v>
       </c>
       <c r="N1562" s="20" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="V1562" s="20"/>
       <c r="W1562" s="4"/>
@@ -45296,7 +45345,7 @@
         <v>213</v>
       </c>
       <c r="N1563" s="20" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="V1563" s="20"/>
       <c r="W1563" s="4"/>
@@ -45324,7 +45373,7 @@
         <v>214</v>
       </c>
       <c r="N1564" s="20" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="S1564" s="2" t="s">
         <v>94</v>
@@ -45355,7 +45404,7 @@
         <v>215</v>
       </c>
       <c r="N1565" s="20" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="V1565" s="20"/>
       <c r="W1565" s="4"/>
@@ -45380,13 +45429,13 @@
         <v>216</v>
       </c>
       <c r="N1566" s="21" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="O1566" s="11" t="s">
         <v>20</v>
       </c>
       <c r="V1566" s="20" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="W1566" s="4"/>
     </row>
@@ -45410,7 +45459,7 @@
         <v>217</v>
       </c>
       <c r="N1567" s="20" t="s">
-        <v>1354</v>
+        <v>1351</v>
       </c>
       <c r="P1567" s="18" t="s">
         <v>66</v>
@@ -45441,7 +45490,7 @@
         <v>218</v>
       </c>
       <c r="N1568" s="21" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="O1568" s="11" t="s">
         <v>21</v>
@@ -45451,7 +45500,7 @@
         <v>93</v>
       </c>
       <c r="V1568" s="20" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="W1568" s="4"/>
     </row>
@@ -45475,7 +45524,7 @@
         <v>219</v>
       </c>
       <c r="N1569" s="21" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="V1569" s="20"/>
       <c r="W1569" s="4"/>
@@ -45500,7 +45549,7 @@
         <v>220</v>
       </c>
       <c r="N1570" s="21" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="O1570" s="11" t="s">
         <v>21</v>
@@ -45508,7 +45557,7 @@
       <c r="T1570" s="29"/>
       <c r="U1570" s="20"/>
       <c r="V1570" s="20" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="W1570" s="4"/>
     </row>
@@ -45532,7 +45581,7 @@
         <v>221</v>
       </c>
       <c r="N1571" s="20" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="T1571" s="29"/>
       <c r="U1571" s="23" t="s">
@@ -45561,7 +45610,7 @@
         <v>222</v>
       </c>
       <c r="N1572" s="20" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="V1572" s="20"/>
       <c r="W1572" s="4"/>
@@ -45586,7 +45635,7 @@
         <v>223</v>
       </c>
       <c r="N1573" s="20" t="s">
-        <v>1355</v>
+        <v>1352</v>
       </c>
       <c r="P1573" s="18" t="s">
         <v>66</v>
@@ -45641,7 +45690,7 @@
         <v>225</v>
       </c>
       <c r="N1575" s="20" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="V1575" s="20"/>
       <c r="W1575" s="4"/>
@@ -45666,7 +45715,7 @@
         <v>226</v>
       </c>
       <c r="N1576" s="20" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="V1576" s="20"/>
       <c r="W1576" s="4"/>
@@ -45676,7 +45725,7 @@
         <v>64</v>
       </c>
       <c r="H1577" s="61" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="I1577" s="4" t="s">
         <v>57</v>
@@ -45694,13 +45743,13 @@
         <v>227</v>
       </c>
       <c r="N1577" s="21" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="O1577" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1577" s="20" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="W1577" s="4"/>
     </row>
@@ -45709,7 +45758,7 @@
         <v>64</v>
       </c>
       <c r="H1578" s="61" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="I1578" s="4" t="s">
         <v>57</v>
@@ -45737,7 +45786,7 @@
         <v>64</v>
       </c>
       <c r="H1579" s="61" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="I1579" s="4" t="s">
         <v>57</v>
@@ -45765,7 +45814,7 @@
         <v>64</v>
       </c>
       <c r="H1580" s="61" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="I1580" s="4" t="s">
         <v>57</v>
@@ -45793,7 +45842,7 @@
         <v>64</v>
       </c>
       <c r="H1581" s="61" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="I1581" s="4" t="s">
         <v>57</v>
@@ -45821,7 +45870,7 @@
         <v>64</v>
       </c>
       <c r="H1582" s="61" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="I1582" s="4" t="s">
         <v>57</v>
@@ -45839,7 +45888,7 @@
         <v>232</v>
       </c>
       <c r="N1582" s="20" t="s">
-        <v>1356</v>
+        <v>1353</v>
       </c>
       <c r="P1582" s="18" t="s">
         <v>66</v>
@@ -45894,7 +45943,7 @@
         <v>234</v>
       </c>
       <c r="N1584" s="20" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="V1584" s="20"/>
       <c r="W1584" s="4"/>
@@ -45919,7 +45968,7 @@
         <v>235</v>
       </c>
       <c r="N1585" s="20" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="V1585" s="20"/>
       <c r="W1585" s="4"/>
@@ -45932,7 +45981,7 @@
         <v>179</v>
       </c>
       <c r="E1586" s="4" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="I1586" s="4" t="s">
         <v>57</v>
@@ -45964,7 +46013,7 @@
         <v>179</v>
       </c>
       <c r="E1587" s="4" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="I1587" s="4" t="s">
         <v>57</v>
@@ -46010,7 +46059,7 @@
         <v>238</v>
       </c>
       <c r="N1588" s="20" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="V1588" s="20"/>
       <c r="W1588" s="4"/>
@@ -46035,7 +46084,7 @@
         <v>239</v>
       </c>
       <c r="N1589" s="20" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="U1589" s="32" t="s">
         <v>68</v>
@@ -46063,13 +46112,13 @@
         <v>240</v>
       </c>
       <c r="N1590" s="21" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="O1590" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1590" s="20" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="W1590" s="4"/>
     </row>
@@ -46093,7 +46142,7 @@
         <v>241</v>
       </c>
       <c r="N1591" s="20" t="s">
-        <v>1357</v>
+        <v>1354</v>
       </c>
       <c r="P1591" s="18" t="s">
         <v>66</v>
@@ -46109,7 +46158,7 @@
         <v>64</v>
       </c>
       <c r="H1592" s="61" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
       <c r="I1592" s="4" t="s">
         <v>57</v>
@@ -46127,7 +46176,7 @@
         <v>242</v>
       </c>
       <c r="N1592" s="20" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="V1592" s="20"/>
       <c r="W1592" s="4"/>
@@ -46137,10 +46186,10 @@
         <v>64</v>
       </c>
       <c r="D1593" s="10" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
       <c r="H1593" s="4" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
       <c r="I1593" s="4" t="s">
         <v>57</v>
@@ -46164,7 +46213,7 @@
         <v>95</v>
       </c>
       <c r="T1593" s="18" t="s">
-        <v>1370</v>
+        <v>1367</v>
       </c>
       <c r="V1593" s="20"/>
       <c r="W1593" s="4"/>
@@ -46174,7 +46223,7 @@
         <v>64</v>
       </c>
       <c r="H1594" s="61" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
       <c r="I1594" s="4" t="s">
         <v>57</v>
@@ -46192,13 +46241,13 @@
         <v>244</v>
       </c>
       <c r="N1594" s="21" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="O1594" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1594" s="20" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="W1594" s="4"/>
     </row>
@@ -46222,13 +46271,13 @@
         <v>245</v>
       </c>
       <c r="N1595" s="21" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="O1595" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1595" s="20" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="W1595" s="4"/>
     </row>
@@ -46252,7 +46301,7 @@
         <v>246</v>
       </c>
       <c r="N1596" s="20" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="V1596" s="20"/>
       <c r="W1596" s="4"/>
@@ -46262,7 +46311,7 @@
         <v>64</v>
       </c>
       <c r="H1597" s="61" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="I1597" s="4" t="s">
         <v>57</v>
@@ -46290,10 +46339,10 @@
         <v>64</v>
       </c>
       <c r="G1598" s="4" t="s">
-        <v>1429</v>
+        <v>1426</v>
       </c>
       <c r="H1598" s="61" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="I1598" s="4" t="s">
         <v>57</v>
@@ -46311,23 +46360,23 @@
         <v>248</v>
       </c>
       <c r="N1598" s="20" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="V1598" s="20"/>
       <c r="W1598" s="4"/>
     </row>
     <row r="1599" spans="2:23" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1599" s="4" t="s">
-        <v>1433</v>
+        <v>1430</v>
       </c>
       <c r="C1599" s="4" t="s">
         <v>64</v>
       </c>
       <c r="G1599" s="4" t="s">
-        <v>1429</v>
+        <v>1426</v>
       </c>
       <c r="H1599" s="61" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="I1599" s="4" t="s">
         <v>57</v>
@@ -46358,10 +46407,10 @@
         <v>64</v>
       </c>
       <c r="G1600" s="4" t="s">
-        <v>1429</v>
+        <v>1426</v>
       </c>
       <c r="H1600" s="61" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="I1600" s="4" t="s">
         <v>57</v>
@@ -46379,7 +46428,7 @@
         <v>250</v>
       </c>
       <c r="N1600" s="20" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="V1600" s="20"/>
       <c r="W1600" s="4"/>
@@ -46389,7 +46438,7 @@
         <v>64</v>
       </c>
       <c r="H1601" s="61" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="I1601" s="4" t="s">
         <v>58</v>
@@ -46407,7 +46456,7 @@
         <v>251</v>
       </c>
       <c r="N1601" s="20" t="s">
-        <v>1358</v>
+        <v>1355</v>
       </c>
       <c r="P1601" s="18" t="s">
         <v>66</v>
@@ -46437,7 +46486,7 @@
         <v>252</v>
       </c>
       <c r="N1602" s="20" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="V1602" s="20"/>
       <c r="W1602" s="4"/>
@@ -46487,13 +46536,13 @@
         <v>254</v>
       </c>
       <c r="N1604" s="21" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="O1604" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1604" s="20" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="W1604" s="4"/>
     </row>
@@ -46517,7 +46566,7 @@
         <v>255</v>
       </c>
       <c r="N1605" s="20" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="V1605" s="20"/>
       <c r="W1605" s="4"/>
@@ -46567,13 +46616,13 @@
         <v>257</v>
       </c>
       <c r="N1607" s="21" t="s">
-        <v>1439</v>
+        <v>1436</v>
       </c>
       <c r="O1607" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1607" s="21" t="s">
-        <v>1440</v>
+        <v>1437</v>
       </c>
       <c r="W1607" s="4"/>
     </row>
@@ -46597,7 +46646,7 @@
         <v>258</v>
       </c>
       <c r="N1608" s="20" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="V1608" s="20"/>
       <c r="W1608" s="4"/>
@@ -46625,7 +46674,7 @@
         <v>259</v>
       </c>
       <c r="N1609" s="20" t="s">
-        <v>1359</v>
+        <v>1356</v>
       </c>
       <c r="P1609" s="18" t="s">
         <v>66</v>
@@ -46656,7 +46705,7 @@
         <v>260</v>
       </c>
       <c r="N1610" s="20" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="V1610" s="20"/>
       <c r="W1610" s="4"/>
@@ -46681,7 +46730,7 @@
         <v>261</v>
       </c>
       <c r="N1611" s="20" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="V1611" s="20"/>
       <c r="W1611" s="4"/>
@@ -46706,7 +46755,7 @@
         <v>262</v>
       </c>
       <c r="N1612" s="20" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="V1612" s="20"/>
       <c r="W1612" s="4"/>
@@ -46731,13 +46780,13 @@
         <v>263</v>
       </c>
       <c r="N1613" s="21" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="O1613" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1613" s="20" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="W1613" s="4"/>
     </row>
@@ -46761,7 +46810,7 @@
         <v>264</v>
       </c>
       <c r="N1614" s="20" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="V1614" s="20"/>
       <c r="W1614" s="4"/>
@@ -46811,7 +46860,7 @@
         <v>266</v>
       </c>
       <c r="N1616" s="20" t="s">
-        <v>1360</v>
+        <v>1357</v>
       </c>
       <c r="P1616" s="18" t="s">
         <v>66</v>
@@ -46826,7 +46875,7 @@
         <v>64</v>
       </c>
       <c r="H1617" s="61" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
       <c r="I1617" s="4" t="s">
         <v>58</v>
@@ -46844,7 +46893,7 @@
         <v>267</v>
       </c>
       <c r="N1617" s="20" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="V1617" s="20"/>
       <c r="W1617" s="4"/>
@@ -46857,10 +46906,10 @@
         <v>179</v>
       </c>
       <c r="E1618" s="4" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="H1618" s="61" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
       <c r="I1618" s="4" t="s">
         <v>58</v>
@@ -46892,10 +46941,10 @@
         <v>179</v>
       </c>
       <c r="E1619" s="4" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="H1619" s="61" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
       <c r="I1619" s="4" t="s">
         <v>58</v>
@@ -46926,7 +46975,7 @@
         <v>64</v>
       </c>
       <c r="H1620" s="61" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
       <c r="I1620" s="4" t="s">
         <v>58</v>
@@ -46944,13 +46993,13 @@
         <v>270</v>
       </c>
       <c r="N1620" s="21" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="O1620" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1620" s="20" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="W1620" s="4"/>
     </row>
@@ -46974,7 +47023,7 @@
         <v>271</v>
       </c>
       <c r="N1621" s="20" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="V1621" s="20"/>
       <c r="W1621" s="4"/>
@@ -47027,7 +47076,7 @@
         <v>273</v>
       </c>
       <c r="N1623" s="20" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="V1623" s="20"/>
       <c r="W1623" s="4"/>
@@ -47052,7 +47101,7 @@
         <v>274</v>
       </c>
       <c r="N1624" s="20" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="V1624" s="20"/>
       <c r="W1624" s="4"/>
@@ -47077,7 +47126,7 @@
         <v>275</v>
       </c>
       <c r="N1625" s="20" t="s">
-        <v>1361</v>
+        <v>1358</v>
       </c>
       <c r="P1625" s="18" t="s">
         <v>66</v>
@@ -47107,7 +47156,7 @@
         <v>276</v>
       </c>
       <c r="N1626" s="20" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="U1626" s="48"/>
       <c r="V1626" s="20"/>
@@ -47133,7 +47182,7 @@
         <v>277</v>
       </c>
       <c r="N1627" s="20" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="U1627" s="48" t="s">
         <v>93</v>
@@ -47239,7 +47288,7 @@
         <v>281</v>
       </c>
       <c r="N1631" s="20" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="V1631" s="20"/>
       <c r="W1631" s="4"/>
@@ -47264,7 +47313,7 @@
         <v>282</v>
       </c>
       <c r="N1632" s="20" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="V1632" s="20"/>
       <c r="W1632" s="4"/>
@@ -47289,14 +47338,14 @@
         <v>283</v>
       </c>
       <c r="N1633" s="21" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="O1633" s="11" t="s">
         <v>21</v>
       </c>
       <c r="U1633" s="48"/>
       <c r="V1633" s="20" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="W1633" s="4"/>
     </row>
@@ -47320,7 +47369,7 @@
         <v>284</v>
       </c>
       <c r="N1634" s="20" t="s">
-        <v>1362</v>
+        <v>1359</v>
       </c>
       <c r="P1634" s="18" t="s">
         <v>66</v>
@@ -47353,13 +47402,13 @@
         <v>285</v>
       </c>
       <c r="N1635" s="21" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="O1635" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1635" s="20" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="W1635" s="4"/>
     </row>
@@ -47383,7 +47432,7 @@
         <v>286</v>
       </c>
       <c r="N1636" s="20" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="V1636" s="20"/>
       <c r="W1636" s="4"/>
@@ -47461,7 +47510,7 @@
         <v>289</v>
       </c>
       <c r="N1639" s="20" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="V1639" s="20"/>
       <c r="W1639" s="4"/>
@@ -47486,7 +47535,7 @@
         <v>290</v>
       </c>
       <c r="N1640" s="20" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="V1640" s="20"/>
       <c r="W1640" s="4"/>
@@ -47539,7 +47588,7 @@
         <v>292</v>
       </c>
       <c r="N1642" s="20" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="V1642" s="20"/>
       <c r="W1642" s="4"/>
@@ -47594,7 +47643,7 @@
         <v>294</v>
       </c>
       <c r="N1644" s="20" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="U1644" s="48"/>
       <c r="V1644" s="20"/>
@@ -47648,13 +47697,13 @@
         <v>296</v>
       </c>
       <c r="N1646" s="21" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="O1646" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1646" s="20" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="W1646" s="4"/>
     </row>
@@ -47678,13 +47727,13 @@
         <v>297</v>
       </c>
       <c r="N1647" s="21" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="O1647" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1647" s="20" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="W1647" s="4"/>
     </row>
@@ -47708,7 +47757,7 @@
         <v>298</v>
       </c>
       <c r="N1648" s="20" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="V1648" s="20"/>
       <c r="W1648" s="4"/>
@@ -47758,7 +47807,7 @@
         <v>300</v>
       </c>
       <c r="N1650" s="20" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="V1650" s="20"/>
       <c r="W1650" s="4"/>
@@ -47783,7 +47832,7 @@
         <v>301</v>
       </c>
       <c r="N1651" s="20" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="V1651" s="20"/>
       <c r="W1651" s="4"/>
@@ -47808,7 +47857,7 @@
         <v>302</v>
       </c>
       <c r="N1652" s="20" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="V1652" s="20"/>
       <c r="W1652" s="4"/>
@@ -47858,7 +47907,7 @@
         <v>304</v>
       </c>
       <c r="N1654" s="20" t="s">
-        <v>1363</v>
+        <v>1360</v>
       </c>
       <c r="P1654" s="18" t="s">
         <v>66</v>
@@ -47916,7 +47965,7 @@
         <v>306</v>
       </c>
       <c r="N1656" s="20" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="V1656" s="20"/>
       <c r="W1656" s="4"/>
@@ -47941,7 +47990,7 @@
         <v>307</v>
       </c>
       <c r="N1657" s="20" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="V1657" s="20"/>
       <c r="W1657" s="4"/>
@@ -47966,7 +48015,7 @@
         <v>308</v>
       </c>
       <c r="N1658" s="20" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="V1658" s="20"/>
       <c r="W1658" s="4"/>
@@ -48066,7 +48115,7 @@
         <v>312</v>
       </c>
       <c r="N1662" s="20" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="V1662" s="20"/>
       <c r="W1662" s="4"/>
@@ -48091,7 +48140,7 @@
         <v>313</v>
       </c>
       <c r="N1663" s="21" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
       <c r="O1663" s="11" t="s">
         <v>21</v>
@@ -48100,7 +48149,7 @@
         <v>66</v>
       </c>
       <c r="V1663" s="20" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="W1663" s="4"/>
     </row>
@@ -48152,7 +48201,7 @@
         <v>315</v>
       </c>
       <c r="N1665" s="20" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="V1665" s="20"/>
       <c r="W1665" s="4"/>
@@ -48177,7 +48226,7 @@
         <v>316</v>
       </c>
       <c r="N1666" s="20" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="V1666" s="20"/>
       <c r="W1666" s="4"/>
@@ -48202,7 +48251,7 @@
         <v>317</v>
       </c>
       <c r="N1667" s="20" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="V1667" s="20"/>
       <c r="W1667" s="4"/>
@@ -48227,13 +48276,13 @@
         <v>318</v>
       </c>
       <c r="N1668" s="21" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="O1668" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1668" s="20" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="W1668" s="4"/>
     </row>
@@ -48257,7 +48306,7 @@
         <v>319</v>
       </c>
       <c r="N1669" s="20" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="V1669" s="20"/>
       <c r="W1669" s="4"/>
@@ -48282,7 +48331,7 @@
         <v>320</v>
       </c>
       <c r="N1670" s="21" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="O1670" s="11" t="s">
         <v>23</v>
@@ -48312,7 +48361,7 @@
         <v>321</v>
       </c>
       <c r="N1671" s="20" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="V1671" s="20"/>
       <c r="W1671" s="4"/>
@@ -48337,7 +48386,7 @@
         <v>322</v>
       </c>
       <c r="N1672" s="21" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
       <c r="O1672" s="11" t="s">
         <v>21</v>
@@ -48346,7 +48395,7 @@
         <v>66</v>
       </c>
       <c r="V1672" s="20" t="s">
-        <v>1367</v>
+        <v>1364</v>
       </c>
       <c r="W1672" s="4"/>
     </row>
@@ -48380,10 +48429,10 @@
         <v>64</v>
       </c>
       <c r="D1674" s="10" t="s">
-        <v>1424</v>
+        <v>1421</v>
       </c>
       <c r="G1674" s="4" t="s">
-        <v>1425</v>
+        <v>1422</v>
       </c>
       <c r="I1674" s="4" t="s">
         <v>59</v>
@@ -48401,7 +48450,7 @@
         <v>324</v>
       </c>
       <c r="N1674" s="20" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="V1674" s="20"/>
       <c r="W1674" s="4"/>
@@ -48411,10 +48460,10 @@
         <v>64</v>
       </c>
       <c r="D1675" s="10" t="s">
-        <v>1424</v>
+        <v>1421</v>
       </c>
       <c r="G1675" s="4" t="s">
-        <v>1425</v>
+        <v>1422</v>
       </c>
       <c r="I1675" s="4" t="s">
         <v>59</v>
@@ -48445,10 +48494,10 @@
         <v>64</v>
       </c>
       <c r="D1676" s="10" t="s">
-        <v>1424</v>
+        <v>1421</v>
       </c>
       <c r="G1676" s="4" t="s">
-        <v>1425</v>
+        <v>1422</v>
       </c>
       <c r="I1676" s="4" t="s">
         <v>59</v>
@@ -48466,7 +48515,7 @@
         <v>326</v>
       </c>
       <c r="N1676" s="20" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="S1676" s="2" t="s">
         <v>97</v>
@@ -48522,13 +48571,13 @@
         <v>328</v>
       </c>
       <c r="N1678" s="21" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="O1678" s="11" t="s">
         <v>21</v>
       </c>
       <c r="V1678" s="20" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="W1678" s="4"/>
     </row>
@@ -48537,7 +48586,7 @@
         <v>64</v>
       </c>
       <c r="H1679" s="61" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="I1679" s="4" t="s">
         <v>59</v>
@@ -48555,7 +48604,7 @@
         <v>329</v>
       </c>
       <c r="N1679" s="20" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="V1679" s="20"/>
       <c r="W1679" s="4"/>
@@ -48565,7 +48614,7 @@
         <v>64</v>
       </c>
       <c r="H1680" s="61" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="I1680" s="4" t="s">
         <v>59</v>
@@ -48583,7 +48632,7 @@
         <v>330</v>
       </c>
       <c r="N1680" s="20" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="V1680" s="20"/>
       <c r="W1680" s="4"/>
@@ -48593,7 +48642,7 @@
         <v>64</v>
       </c>
       <c r="H1681" s="61" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="I1681" s="4" t="s">
         <v>59</v>
@@ -48626,7 +48675,7 @@
         <v>64</v>
       </c>
       <c r="H1682" s="61" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="I1682" s="4" t="s">
         <v>59</v>
@@ -48644,7 +48693,7 @@
         <v>332</v>
       </c>
       <c r="N1682" s="20" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="V1682" s="20"/>
       <c r="W1682" s="4"/>
@@ -48654,7 +48703,7 @@
         <v>64</v>
       </c>
       <c r="H1683" s="61" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="I1683" s="4" t="s">
         <v>59</v>
@@ -48672,7 +48721,7 @@
         <v>333</v>
       </c>
       <c r="N1683" s="20" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="V1683" s="20"/>
       <c r="W1683" s="4"/>
@@ -48682,7 +48731,7 @@
         <v>64</v>
       </c>
       <c r="H1684" s="61" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="I1684" s="4" t="s">
         <v>59</v>
@@ -48710,7 +48759,7 @@
         <v>64</v>
       </c>
       <c r="H1685" s="61" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="I1685" s="4" t="s">
         <v>59</v>
@@ -48741,7 +48790,7 @@
         <v>64</v>
       </c>
       <c r="H1686" s="61" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="I1686" s="4" t="s">
         <v>59</v>
@@ -48759,7 +48808,7 @@
         <v>336</v>
       </c>
       <c r="N1686" s="20" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="V1686" s="20"/>
       <c r="W1686" s="4"/>
@@ -48784,7 +48833,7 @@
         <v>337</v>
       </c>
       <c r="N1687" s="20" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="V1687" s="20"/>
       <c r="W1687" s="4"/>
@@ -48834,7 +48883,7 @@
         <v>339</v>
       </c>
       <c r="N1689" s="20" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="V1689" s="20"/>
       <c r="W1689" s="4"/>
@@ -48859,14 +48908,14 @@
         <v>340</v>
       </c>
       <c r="N1690" s="21" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="O1690" s="11" t="s">
         <v>21</v>
       </c>
       <c r="U1690" s="20"/>
       <c r="V1690" s="20" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="W1690" s="4"/>
     </row>
@@ -48890,7 +48939,7 @@
         <v>341</v>
       </c>
       <c r="N1691" s="20" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="P1691" s="18" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
nmv 30 04 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.2 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D14F80-83E7-4528-BBB3-3E2A3ED96DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFD208E-A188-40A9-9B4D-C70DBB392A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5259,9 +5259,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1691"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1258" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V1261" sqref="V1261"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A585" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F586" sqref="F586"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20494,8 +20494,8 @@
       <c r="M593" s="7">
         <v>74</v>
       </c>
-      <c r="N593" s="20" t="s">
-        <v>287</v>
+      <c r="N593" s="21" t="s">
+        <v>201</v>
       </c>
       <c r="V593" s="20"/>
       <c r="W593" s="4"/>

</xml_diff>